<commit_message>
ux upgrade + default nbh excel change
</commit_message>
<xml_diff>
--- a/data_ProjectTemplate/Neighbourhoods_ProjectTemplate.xlsx
+++ b/data_ProjectTemplate/Neighbourhoods_ProjectTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AteHe\Desktop\Modellen\Zero_ProjectTemplate\data_ProjectTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AteHe\Desktop\Modellen\LUX_ProjectTemplate\data_ProjectTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ECAAAD-0009-4D07-88E9-CDF040BEF4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FDCA02-75E0-40D5-AB3D-F38343D76A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="neighbourhoods" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Luc Sol:</t>
         </r>
@@ -47,7 +47,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 String (mandatory)
@@ -63,7 +63,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Luc Sol:</t>
         </r>
@@ -72,7 +72,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 String (optional)
@@ -88,7 +88,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Luc Sol:</t>
         </r>
@@ -97,7 +97,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 String (optional)</t>
@@ -112,7 +112,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Luc Sol:</t>
         </r>
@@ -121,7 +121,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 String (mandatory)
@@ -129,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{A81BA535-2E73-4AED-B40E-7FCFC7DCA2DB}">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{A81BA535-2E73-4AED-B40E-7FCFC7DCA2DB}">
       <text>
         <r>
           <rPr>
@@ -137,7 +137,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Luc Sol:</t>
         </r>
@@ -146,7 +146,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 double (mandatory)
@@ -154,7 +154,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{FC11B76F-766B-458F-9BA6-E40AB8864725}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{FC11B76F-766B-458F-9BA6-E40AB8864725}">
       <text>
         <r>
           <rPr>
@@ -162,7 +162,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Luc Sol:</t>
         </r>
@@ -171,7 +171,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 double (mandatory)
@@ -179,7 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{BF765C18-B9EC-4738-8EE6-79B3BE290F90}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{BF765C18-B9EC-4738-8EE6-79B3BE290F90}">
       <text>
         <r>
           <rPr>
@@ -187,7 +187,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Luc Sol:</t>
         </r>
@@ -196,7 +196,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 String (mandatory)
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>latitude</t>
   </si>
@@ -246,6 +246,30 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>avg_number_of_cars_per_house</t>
+  </si>
+  <si>
+    <t>total_nr_comp_cars</t>
+  </si>
+  <si>
+    <t>total_nr_comp_vans</t>
+  </si>
+  <si>
+    <t>total_nr_comp_trucks</t>
+  </si>
+  <si>
+    <t>avg_house_elec_delivery_kwh_p_yr</t>
+  </si>
+  <si>
+    <t>total_comp_elec_delivery_kwh_p_yr</t>
+  </si>
+  <si>
+    <t>total_comp_gas_delivery_m3_p_yr</t>
+  </si>
+  <si>
+    <t>avg_house_gas_delivery_m3_p_yr</t>
   </si>
 </sst>
 </file>
@@ -264,14 +288,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -282,94 +306,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -387,64 +329,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -727,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -739,97 +634,145 @@
     <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="28" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="34" max="40" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="4.81640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="42.81640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="48" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.26953125" customWidth="1"/>
+    <col min="6" max="6" width="30.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="255.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="29" max="36" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="40" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="42" max="48" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="42.81640625" bestFit="1" customWidth="1"/>
+    <col min="55" max="56" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="15.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="3">
         <v>0</v>
       </c>
-      <c r="F2" s="5">
+      <c r="N2" s="3">
         <v>0</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="O2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="8">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
         <v>666</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="3">
         <v>0</v>
       </c>
-      <c r="F3" s="9">
+      <c r="N3" s="3">
         <v>0</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="O3" s="3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
preliminary updates for nbh code refactor of interface
</commit_message>
<xml_diff>
--- a/data_ProjectTemplate/Neighbourhoods_ProjectTemplate.xlsx
+++ b/data_ProjectTemplate/Neighbourhoods_ProjectTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AteHe\Desktop\Modellen\LUX_ProjectTemplate\data_ProjectTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FDCA02-75E0-40D5-AB3D-F38343D76A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB942C88-210F-4BCA-92FA-9D31583A3EC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -227,9 +227,6 @@
     <t>districtcode</t>
   </si>
   <si>
-    <t>districtname</t>
-  </si>
-  <si>
     <t>neighbourhoodcode</t>
   </si>
   <si>
@@ -270,6 +267,9 @@
   </si>
   <si>
     <t>avg_house_gas_delivery_m3_p_yr</t>
+  </si>
+  <si>
+    <t>neighbourhoodname</t>
   </si>
 </sst>
 </file>
@@ -625,15 +625,15 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.26953125" customWidth="1"/>
     <col min="6" max="6" width="30.36328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29" bestFit="1" customWidth="1"/>
@@ -673,40 +673,40 @@
   <sheetData>
     <row r="1" spans="1:15" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>7</v>
-      </c>
       <c r="E1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>0</v>
@@ -720,14 +720,14 @@
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -744,7 +744,7 @@
         <v>0</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -756,7 +756,7 @@
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -773,7 +773,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>